<commit_message>
indivual buttons for each digit
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4129" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4453" uniqueCount="151">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -500,6 +500,27 @@
   </si>
   <si>
     <t xml:space="preserve">0.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;FVAL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency  [Hertz]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phase inc: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543.210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFEEDDCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back</t>
   </si>
 </sst>
 </file>
@@ -2038,13 +2059,13 @@
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
@@ -2061,7 +2082,7 @@
         <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6">
@@ -2112,7 +2133,7 @@
         <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9">
@@ -2151,10 +2172,10 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -2163,15 +2184,15 @@
         <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
@@ -2180,12 +2201,12 @@
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
         <v>90</v>
@@ -2197,15 +2218,15 @@
         <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -2214,15 +2235,15 @@
         <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -2231,15 +2252,15 @@
         <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
         <v>47</v>
@@ -2248,12 +2269,12 @@
         <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
@@ -2265,15 +2286,15 @@
         <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
@@ -2282,15 +2303,15 @@
         <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
@@ -2299,12 +2320,12 @@
         <v>48</v>
       </c>
       <c r="F19" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
         <v>45</v>
@@ -2316,15 +2337,15 @@
         <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
         <v>47</v>
@@ -2333,26 +2354,10 @@
         <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="s">
-        <v>141</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" t="s">
-        <v>142</v>
-      </c>
-    </row>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22"/>
     <row r="23"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>